<commit_message>
Updated report structure and finished 5 epochs
</commit_message>
<xml_diff>
--- a/Report/structure.xlsx
+++ b/Report/structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippmetzger/Documents/GitHub/Deep_Learning_Project_Group_10/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D0C341-5900-E249-B67E-64A3BC2B426C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B6368C-99C9-B646-8710-9404AB3D3086}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33080" yWindow="2860" windowWidth="28040" windowHeight="16420" xr2:uid="{34E6199A-B0D9-7A43-AB7C-E184A4B441F3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>DL Group project report structure</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Error analysis (If and what not yet decided)</t>
+  </si>
+  <si>
+    <t>Maximun number of pages (whole chapter)</t>
   </si>
 </sst>
 </file>
@@ -120,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -128,12 +131,141 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7514C459-D3A4-7D42-95A4-B574ED084ECC}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,91 +591,128 @@
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D4" s="11">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated report structure file
</commit_message>
<xml_diff>
--- a/Report/structure.xlsx
+++ b/Report/structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippmetzger/Documents/GitHub/Deep_Learning_Project_Group_10/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77DDCB2-9882-6745-95FD-6848394BB7FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC87126-77C1-BD44-91E0-E55CE6EF6301}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33080" yWindow="2860" windowWidth="28040" windowHeight="16420" xr2:uid="{34E6199A-B0D9-7A43-AB7C-E184A4B441F3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27300" windowHeight="16380" xr2:uid="{34E6199A-B0D9-7A43-AB7C-E184A4B441F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>DL Group project report structure</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Maximun number of pages (whole chapter)</t>
+  </si>
+  <si>
+    <t>Philipp</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,7 +634,9 @@
       <c r="D4" s="11">
         <v>1</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Added photographs of traffic signs and 'Meta' images. Also updated report structure file
</commit_message>
<xml_diff>
--- a/Report/structure.xlsx
+++ b/Report/structure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippmetzger/Documents/GitHub/Deep_Learning_Project_Group_10/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936FEFD9-8F40-F64E-8156-23DFAF61970E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97833D67-C988-4148-8D14-D25403E531B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27300" windowHeight="16280" xr2:uid="{34E6199A-B0D9-7A43-AB7C-E184A4B441F3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27300" windowHeight="16280" xr2:uid="{34E6199A-B0D9-7A43-AB7C-E184A4B441F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>DL Group project report structure</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>Franz</t>
+  </si>
+  <si>
+    <t>Subchapter No.</t>
+  </si>
+  <si>
+    <t>i.</t>
+  </si>
+  <si>
+    <t>ii.</t>
+  </si>
+  <si>
+    <t>iii.</t>
+  </si>
+  <si>
+    <t>iv.</t>
   </si>
 </sst>
 </file>
@@ -258,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -272,9 +287,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -290,7 +306,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -586,28 +602,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7514C459-D3A4-7D42-95A4-B574ED084ECC}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -615,33 +631,37 @@
         <v>4</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11">
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -649,47 +669,61 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" s="8"/>
+      <c r="F8" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -697,36 +731,43 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="11">
+      <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>